<commit_message>
work added to time-tracker
</commit_message>
<xml_diff>
--- a/time-tracker.xlsx
+++ b/time-tracker.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FED1A08-C6B1-47B1-BF43-28AB355A7657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>MINUTES</t>
   </si>
@@ -83,12 +84,33 @@
   </si>
   <si>
     <t>Build working prototype</t>
+  </si>
+  <si>
+    <t>https://github.com/chat-loc/chatloc.github.io/commit/a28fef4d8582293946dbff07fa83c1827432158f</t>
+  </si>
+  <si>
+    <t>Creating chat user interface</t>
+  </si>
+  <si>
+    <t>Khushboo</t>
+  </si>
+  <si>
+    <t>https://github.com/chat-loc/chatloc.github.io/pull/26/commits/3398a9cf0b0f7920890fe363bfc6e728045f48c7</t>
+  </si>
+  <si>
+    <t>Created landing page, css files and login page</t>
+  </si>
+  <si>
+    <t>https://github.com/chat-loc/chatloc.github.io/commit/a45398dcb5d9e7db44ce3e49223b552742ae46c3</t>
+  </si>
+  <si>
+    <t>Making login logout and room list responsive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,6 +267,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -280,6 +319,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,26 +511,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="92" style="2" customWidth="1"/>
-    <col min="8" max="8" width="109.140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="109.109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -491,7 +548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -508,7 +565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -525,7 +582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -542,7 +599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -559,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -576,7 +633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -593,7 +650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -610,7 +667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -627,7 +684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -644,19 +701,73 @@
         <v>22</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4">
+        <v>44023</v>
+      </c>
+      <c r="E12" s="2">
+        <v>450</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4">
+        <v>44032</v>
+      </c>
+      <c r="E13" s="2">
+        <v>400</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4">
+        <v>44014</v>
+      </c>
+      <c r="E14" s="2">
+        <v>390</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G4" r:id="rId2"/>
-    <hyperlink ref="G5" r:id="rId3"/>
-    <hyperlink ref="G6" r:id="rId4"/>
-    <hyperlink ref="G7" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G9" r:id="rId7"/>
-    <hyperlink ref="G10" r:id="rId8"/>
-    <hyperlink ref="G11" r:id="rId9"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{8B7909D2-6BEC-4DC4-A3E6-83C94855DB76}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{6B4A4869-0BA1-4FE6-860D-648BEC983EAE}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{C815495F-6B54-4033-B864-0AB9DDD24A0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
time-tracker file updated. work hours added to the file
</commit_message>
<xml_diff>
--- a/time-tracker.xlsx
+++ b/time-tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FED1A08-C6B1-47B1-BF43-28AB355A7657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE242876-BE71-4FC8-9F13-65C599BA7315}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>MINUTES</t>
   </si>
@@ -104,7 +104,22 @@
     <t>https://github.com/chat-loc/chatloc.github.io/commit/a45398dcb5d9e7db44ce3e49223b552742ae46c3</t>
   </si>
   <si>
-    <t>Making login logout and room list responsive</t>
+    <t>https://github.com/chat-loc/chatloc.github.io/commit/286ca9c3a8555e0c7234327dfac620043f4d2921</t>
+  </si>
+  <si>
+    <t>https://github.com/chat-loc/chatloc.github.io/commit/fa82cd20851166d39e7316799dab1363fe4a4404</t>
+  </si>
+  <si>
+    <t>Making login logout and room list responsive with Aman</t>
+  </si>
+  <si>
+    <t>dark mode theme with Aman</t>
+  </si>
+  <si>
+    <t>merging the dark mode theme to master branch with Aman</t>
+  </si>
+  <si>
+    <t>Khushboo / Aman</t>
   </si>
 </sst>
 </file>
@@ -512,15 +527,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.109375" style="2" customWidth="1"/>
@@ -737,7 +752,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4">
         <v>44014</v>
@@ -749,7 +764,41 @@
         <v>28</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44050</v>
+      </c>
+      <c r="E15" s="2">
+        <v>250</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>29</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="4">
+        <v>44051</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -766,8 +815,10 @@
     <hyperlink ref="G12" r:id="rId10" xr:uid="{8B7909D2-6BEC-4DC4-A3E6-83C94855DB76}"/>
     <hyperlink ref="G13" r:id="rId11" xr:uid="{6B4A4869-0BA1-4FE6-860D-648BEC983EAE}"/>
     <hyperlink ref="G14" r:id="rId12" xr:uid="{C815495F-6B54-4033-B864-0AB9DDD24A0C}"/>
+    <hyperlink ref="G15" r:id="rId13" xr:uid="{838E5276-EFE4-4AB6-9D19-E2DDD6BDE60D}"/>
+    <hyperlink ref="G16" r:id="rId14" xr:uid="{A9BB5117-1889-46FE-B16F-2AE07B15FE06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change 'road' to 'path' due to opencagedata API change; address environment misbehaviour in Heroku
</commit_message>
<xml_diff>
--- a/time-tracker.xlsx
+++ b/time-tracker.xlsx
@@ -58,9 +58,6 @@
     <t>Create Login module</t>
   </si>
   <si>
-    <t>Design Registration module and introduced project theme</t>
-  </si>
-  <si>
     <t>https://github.com/chat-loc/chatloc.github.io/commit/20e1f9174e1e0fe7a9632a09e14cce2207b1dbb9</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Convert app to React II (Heroku MERN Deployment Reconfig)</t>
+  </si>
+  <si>
+    <t>Design Registration module and introduce project theme</t>
   </si>
 </sst>
 </file>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -591,7 +591,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -673,10 +673,10 @@
         <v>200</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -690,10 +690,10 @@
         <v>400</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -707,10 +707,10 @@
         <v>85</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -724,10 +724,10 @@
         <v>400</v>
       </c>
       <c r="G11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -738,10 +738,10 @@
         <v>44028</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -752,10 +752,10 @@
         <v>44028</v>
       </c>
       <c r="G13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -768,7 +768,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4">
         <v>44023</v>
@@ -777,15 +777,15 @@
         <v>450</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4">
         <v>44032</v>
@@ -794,15 +794,15 @@
         <v>400</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4">
         <v>44014</v>
@@ -811,15 +811,15 @@
         <v>390</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4">
         <v>44050</v>
@@ -828,15 +828,15 @@
         <v>250</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="4">
         <v>44051</v>
@@ -845,15 +845,15 @@
         <v>10</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="8">
@@ -866,12 +866,12 @@
       <c r="F24" s="6"/>
       <c r="G24" s="9"/>
       <c r="H24" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="8">
@@ -883,15 +883,15 @@
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="8">
@@ -903,15 +903,15 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="8">
@@ -923,15 +923,15 @@
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C28" s="8">
         <v>44017</v>
@@ -940,15 +940,15 @@
         <v>200</v>
       </c>
       <c r="G28" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="8">
         <v>44018</v>
@@ -957,15 +957,15 @@
         <v>150</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="8">
         <v>44018</v>
@@ -974,10 +974,10 @@
         <v>120</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>